<commit_message>
Update 23 SEPTEMBER - 28 SEPTEMBER.xlsx
</commit_message>
<xml_diff>
--- a/STOCK UTN/23 SEPTEMBER - 28 SEPTEMBER.xlsx
+++ b/STOCK UTN/23 SEPTEMBER - 28 SEPTEMBER.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" showInkAnnotation="0" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="5055" yWindow="1035" windowWidth="10455" windowHeight="10800" tabRatio="803" activeTab="3"/>
+    <workbookView xWindow="5055" yWindow="1035" windowWidth="10455" windowHeight="10800" tabRatio="803" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="JK KENKO" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7815" uniqueCount="3833">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7721" uniqueCount="3832">
   <si>
     <t>Abjad Magnit K B 8125</t>
   </si>
@@ -11553,9 +11553,6 @@
   </si>
   <si>
     <t>MAP-SK217</t>
-  </si>
-  <si>
-    <t>GLOBAL</t>
   </si>
 </sst>
 </file>
@@ -11794,9 +11791,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -11807,6 +11801,9 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Neutral" xfId="4" builtinId="28"/>
@@ -11815,27 +11812,7 @@
     <cellStyle name="常规 2" xfId="3"/>
     <cellStyle name="常规 3" xfId="2"/>
   </cellStyles>
-  <dxfs count="11">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="9">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -12503,10 +12480,10 @@
       <c r="B1" s="8"/>
     </row>
     <row r="2" spans="1:4" ht="12.75" customHeight="1">
-      <c r="A2" s="31" t="s">
+      <c r="A2" s="30" t="s">
         <v>2655</v>
       </c>
-      <c r="B2" s="32"/>
+      <c r="B2" s="31"/>
       <c r="C2" s="7">
         <v>1</v>
       </c>
@@ -12515,10 +12492,10 @@
       </c>
     </row>
     <row r="3" spans="1:4" ht="12.75" customHeight="1">
-      <c r="A3" s="31" t="s">
+      <c r="A3" s="30" t="s">
         <v>3156</v>
       </c>
-      <c r="B3" s="32"/>
+      <c r="B3" s="31"/>
       <c r="C3" s="7">
         <v>1</v>
       </c>
@@ -12527,10 +12504,10 @@
       </c>
     </row>
     <row r="4" spans="1:4" ht="12.75" customHeight="1">
-      <c r="A4" s="31" t="s">
+      <c r="A4" s="30" t="s">
         <v>2656</v>
       </c>
-      <c r="B4" s="32"/>
+      <c r="B4" s="31"/>
       <c r="C4" s="7">
         <v>1</v>
       </c>
@@ -12539,10 +12516,10 @@
       </c>
     </row>
     <row r="5" spans="1:4" ht="12.75" customHeight="1">
-      <c r="A5" s="31" t="s">
+      <c r="A5" s="30" t="s">
         <v>2657</v>
       </c>
-      <c r="B5" s="32"/>
+      <c r="B5" s="31"/>
       <c r="C5" s="7">
         <v>4</v>
       </c>
@@ -12551,10 +12528,10 @@
       </c>
     </row>
     <row r="6" spans="1:4" ht="12.75" customHeight="1">
-      <c r="A6" s="31" t="s">
+      <c r="A6" s="30" t="s">
         <v>2860</v>
       </c>
-      <c r="B6" s="32"/>
+      <c r="B6" s="31"/>
       <c r="C6" s="7">
         <v>2</v>
       </c>
@@ -12563,10 +12540,10 @@
       </c>
     </row>
     <row r="7" spans="1:4" ht="12.75" customHeight="1">
-      <c r="A7" s="31" t="s">
+      <c r="A7" s="30" t="s">
         <v>2861</v>
       </c>
-      <c r="B7" s="32"/>
+      <c r="B7" s="31"/>
       <c r="C7" s="7">
         <v>1</v>
       </c>
@@ -12575,10 +12552,10 @@
       </c>
     </row>
     <row r="8" spans="1:4" ht="12.75" customHeight="1">
-      <c r="A8" s="31" t="s">
+      <c r="A8" s="30" t="s">
         <v>2549</v>
       </c>
-      <c r="B8" s="32"/>
+      <c r="B8" s="31"/>
       <c r="C8" s="7">
         <v>2</v>
       </c>
@@ -12587,10 +12564,10 @@
       </c>
     </row>
     <row r="9" spans="1:4" ht="12.75" customHeight="1">
-      <c r="A9" s="31" t="s">
+      <c r="A9" s="30" t="s">
         <v>3037</v>
       </c>
-      <c r="B9" s="32"/>
+      <c r="B9" s="31"/>
       <c r="C9" s="7">
         <v>1</v>
       </c>
@@ -12599,10 +12576,10 @@
       </c>
     </row>
     <row r="10" spans="1:4" ht="12.75" customHeight="1">
-      <c r="A10" s="31" t="s">
+      <c r="A10" s="30" t="s">
         <v>3038</v>
       </c>
-      <c r="B10" s="32"/>
+      <c r="B10" s="31"/>
       <c r="C10" s="7">
         <v>1</v>
       </c>
@@ -12611,10 +12588,10 @@
       </c>
     </row>
     <row r="11" spans="1:4" ht="12.75" customHeight="1">
-      <c r="A11" s="31" t="s">
+      <c r="A11" s="30" t="s">
         <v>3039</v>
       </c>
-      <c r="B11" s="32"/>
+      <c r="B11" s="31"/>
       <c r="C11" s="7">
         <v>1</v>
       </c>
@@ -12623,10 +12600,10 @@
       </c>
     </row>
     <row r="12" spans="1:4" ht="12.75" customHeight="1">
-      <c r="A12" s="31" t="s">
+      <c r="A12" s="30" t="s">
         <v>3040</v>
       </c>
-      <c r="B12" s="32"/>
+      <c r="B12" s="31"/>
       <c r="C12" s="7">
         <v>1</v>
       </c>
@@ -12635,10 +12612,10 @@
       </c>
     </row>
     <row r="13" spans="1:4" ht="12.75" customHeight="1">
-      <c r="A13" s="31" t="s">
+      <c r="A13" s="30" t="s">
         <v>2862</v>
       </c>
-      <c r="B13" s="32"/>
+      <c r="B13" s="31"/>
       <c r="C13" s="7">
         <v>1</v>
       </c>
@@ -12647,10 +12624,10 @@
       </c>
     </row>
     <row r="14" spans="1:4" ht="12.75" customHeight="1">
-      <c r="A14" s="31" t="s">
+      <c r="A14" s="30" t="s">
         <v>2863</v>
       </c>
-      <c r="B14" s="32"/>
+      <c r="B14" s="31"/>
       <c r="C14" s="7">
         <v>1</v>
       </c>
@@ -12659,10 +12636,10 @@
       </c>
     </row>
     <row r="15" spans="1:4" ht="12.75" customHeight="1">
-      <c r="A15" s="31" t="s">
+      <c r="A15" s="30" t="s">
         <v>3803</v>
       </c>
-      <c r="B15" s="32"/>
+      <c r="B15" s="31"/>
       <c r="C15" s="7">
         <v>117</v>
       </c>
@@ -12671,10 +12648,10 @@
       </c>
     </row>
     <row r="16" spans="1:4" ht="12.75" customHeight="1">
-      <c r="A16" s="31" t="s">
+      <c r="A16" s="30" t="s">
         <v>2658</v>
       </c>
-      <c r="B16" s="32"/>
+      <c r="B16" s="31"/>
       <c r="C16" s="7">
         <v>1</v>
       </c>
@@ -12683,10 +12660,10 @@
       </c>
     </row>
     <row r="17" spans="1:4" ht="12.75" customHeight="1">
-      <c r="A17" s="31" t="s">
+      <c r="A17" s="30" t="s">
         <v>2659</v>
       </c>
-      <c r="B17" s="32"/>
+      <c r="B17" s="31"/>
       <c r="C17" s="7">
         <v>5</v>
       </c>
@@ -12695,10 +12672,10 @@
       </c>
     </row>
     <row r="18" spans="1:4" ht="12.75" customHeight="1">
-      <c r="A18" s="31" t="s">
+      <c r="A18" s="30" t="s">
         <v>2777</v>
       </c>
-      <c r="B18" s="32"/>
+      <c r="B18" s="31"/>
       <c r="C18" s="7">
         <v>1</v>
       </c>
@@ -12707,10 +12684,10 @@
       </c>
     </row>
     <row r="19" spans="1:4" ht="12.75" customHeight="1">
-      <c r="A19" s="31" t="s">
+      <c r="A19" s="30" t="s">
         <v>2469</v>
       </c>
-      <c r="B19" s="32"/>
+      <c r="B19" s="31"/>
       <c r="C19" s="7">
         <v>1</v>
       </c>
@@ -12719,10 +12696,10 @@
       </c>
     </row>
     <row r="20" spans="1:4" ht="12.75" customHeight="1">
-      <c r="A20" s="31" t="s">
+      <c r="A20" s="30" t="s">
         <v>2568</v>
       </c>
-      <c r="B20" s="32"/>
+      <c r="B20" s="31"/>
       <c r="C20" s="7">
         <v>2</v>
       </c>
@@ -12731,10 +12708,10 @@
       </c>
     </row>
     <row r="21" spans="1:4" ht="12.75" customHeight="1">
-      <c r="A21" s="31" t="s">
+      <c r="A21" s="30" t="s">
         <v>2470</v>
       </c>
-      <c r="B21" s="32"/>
+      <c r="B21" s="31"/>
       <c r="C21" s="7">
         <v>1</v>
       </c>
@@ -12743,10 +12720,10 @@
       </c>
     </row>
     <row r="22" spans="1:4" ht="12.75" customHeight="1">
-      <c r="A22" s="31" t="s">
+      <c r="A22" s="30" t="s">
         <v>2471</v>
       </c>
-      <c r="B22" s="32"/>
+      <c r="B22" s="31"/>
       <c r="C22" s="7">
         <v>7</v>
       </c>
@@ -12755,10 +12732,10 @@
       </c>
     </row>
     <row r="23" spans="1:4" ht="12.75" customHeight="1">
-      <c r="A23" s="31" t="s">
+      <c r="A23" s="30" t="s">
         <v>485</v>
       </c>
-      <c r="B23" s="32"/>
+      <c r="B23" s="31"/>
       <c r="C23" s="7">
         <v>26</v>
       </c>
@@ -12767,10 +12744,10 @@
       </c>
     </row>
     <row r="24" spans="1:4" ht="12.75" customHeight="1">
-      <c r="A24" s="31" t="s">
+      <c r="A24" s="30" t="s">
         <v>486</v>
       </c>
-      <c r="B24" s="32"/>
+      <c r="B24" s="31"/>
       <c r="C24" s="7">
         <v>11</v>
       </c>
@@ -12779,10 +12756,10 @@
       </c>
     </row>
     <row r="25" spans="1:4" ht="12.75" customHeight="1">
-      <c r="A25" s="31" t="s">
+      <c r="A25" s="30" t="s">
         <v>2550</v>
       </c>
-      <c r="B25" s="32"/>
+      <c r="B25" s="31"/>
       <c r="C25" s="7">
         <v>3</v>
       </c>
@@ -12791,10 +12768,10 @@
       </c>
     </row>
     <row r="26" spans="1:4" ht="12.75" customHeight="1">
-      <c r="A26" s="31" t="s">
+      <c r="A26" s="30" t="s">
         <v>487</v>
       </c>
-      <c r="B26" s="32"/>
+      <c r="B26" s="31"/>
       <c r="C26" s="7">
         <v>20</v>
       </c>
@@ -12803,10 +12780,10 @@
       </c>
     </row>
     <row r="27" spans="1:4" ht="12.75" customHeight="1">
-      <c r="A27" s="31" t="s">
+      <c r="A27" s="30" t="s">
         <v>2660</v>
       </c>
-      <c r="B27" s="32"/>
+      <c r="B27" s="31"/>
       <c r="C27" s="7">
         <v>2</v>
       </c>
@@ -12815,10 +12792,10 @@
       </c>
     </row>
     <row r="28" spans="1:4" ht="12.75" customHeight="1">
-      <c r="A28" s="31" t="s">
+      <c r="A28" s="30" t="s">
         <v>488</v>
       </c>
-      <c r="B28" s="32"/>
+      <c r="B28" s="31"/>
       <c r="C28" s="7">
         <v>1</v>
       </c>
@@ -12827,10 +12804,10 @@
       </c>
     </row>
     <row r="29" spans="1:4" ht="12.75" customHeight="1">
-      <c r="A29" s="31" t="s">
+      <c r="A29" s="30" t="s">
         <v>489</v>
       </c>
-      <c r="B29" s="32"/>
+      <c r="B29" s="31"/>
       <c r="C29" s="7">
         <v>18</v>
       </c>
@@ -12839,10 +12816,10 @@
       </c>
     </row>
     <row r="30" spans="1:4" ht="12.75" customHeight="1">
-      <c r="A30" s="31" t="s">
+      <c r="A30" s="30" t="s">
         <v>2661</v>
       </c>
-      <c r="B30" s="32"/>
+      <c r="B30" s="31"/>
       <c r="C30" s="7">
         <v>4</v>
       </c>
@@ -12851,10 +12828,10 @@
       </c>
     </row>
     <row r="31" spans="1:4" ht="12.75" customHeight="1">
-      <c r="A31" s="31" t="s">
+      <c r="A31" s="30" t="s">
         <v>2662</v>
       </c>
-      <c r="B31" s="32"/>
+      <c r="B31" s="31"/>
       <c r="C31" s="7">
         <v>13</v>
       </c>
@@ -12863,10 +12840,10 @@
       </c>
     </row>
     <row r="32" spans="1:4" ht="12.75" customHeight="1">
-      <c r="A32" s="31" t="s">
+      <c r="A32" s="30" t="s">
         <v>3537</v>
       </c>
-      <c r="B32" s="32"/>
+      <c r="B32" s="31"/>
       <c r="C32" s="7">
         <v>3</v>
       </c>
@@ -12875,10 +12852,10 @@
       </c>
     </row>
     <row r="33" spans="1:4" ht="12.75" customHeight="1">
-      <c r="A33" s="31" t="s">
+      <c r="A33" s="30" t="s">
         <v>3538</v>
       </c>
-      <c r="B33" s="32"/>
+      <c r="B33" s="31"/>
       <c r="C33" s="7">
         <v>3</v>
       </c>
@@ -12887,10 +12864,10 @@
       </c>
     </row>
     <row r="34" spans="1:4" ht="12.75" customHeight="1">
-      <c r="A34" s="31" t="s">
+      <c r="A34" s="30" t="s">
         <v>2821</v>
       </c>
-      <c r="B34" s="32"/>
+      <c r="B34" s="31"/>
       <c r="C34" s="7">
         <v>4</v>
       </c>
@@ -12899,10 +12876,10 @@
       </c>
     </row>
     <row r="35" spans="1:4" ht="12.75" customHeight="1">
-      <c r="A35" s="31" t="s">
+      <c r="A35" s="30" t="s">
         <v>490</v>
       </c>
-      <c r="B35" s="32"/>
+      <c r="B35" s="31"/>
       <c r="C35" s="7">
         <v>5</v>
       </c>
@@ -12911,10 +12888,10 @@
       </c>
     </row>
     <row r="36" spans="1:4" ht="12.75" customHeight="1">
-      <c r="A36" s="31" t="s">
+      <c r="A36" s="30" t="s">
         <v>2701</v>
       </c>
-      <c r="B36" s="32"/>
+      <c r="B36" s="31"/>
       <c r="C36" s="7">
         <v>1</v>
       </c>
@@ -12923,10 +12900,10 @@
       </c>
     </row>
     <row r="37" spans="1:4" ht="12.75" customHeight="1">
-      <c r="A37" s="31" t="s">
+      <c r="A37" s="30" t="s">
         <v>2663</v>
       </c>
-      <c r="B37" s="32"/>
+      <c r="B37" s="31"/>
       <c r="C37" s="7">
         <v>54</v>
       </c>
@@ -12935,10 +12912,10 @@
       </c>
     </row>
     <row r="38" spans="1:4" ht="12.75" customHeight="1">
-      <c r="A38" s="31" t="s">
+      <c r="A38" s="30" t="s">
         <v>2714</v>
       </c>
-      <c r="B38" s="32"/>
+      <c r="B38" s="31"/>
       <c r="C38" s="7">
         <v>2</v>
       </c>
@@ -12947,10 +12924,10 @@
       </c>
     </row>
     <row r="39" spans="1:4" ht="12.75" customHeight="1">
-      <c r="A39" s="31" t="s">
+      <c r="A39" s="30" t="s">
         <v>2822</v>
       </c>
-      <c r="B39" s="32"/>
+      <c r="B39" s="31"/>
       <c r="C39" s="7">
         <v>3</v>
       </c>
@@ -12959,10 +12936,10 @@
       </c>
     </row>
     <row r="40" spans="1:4" ht="12.75" customHeight="1">
-      <c r="A40" s="31" t="s">
+      <c r="A40" s="30" t="s">
         <v>2664</v>
       </c>
-      <c r="B40" s="32"/>
+      <c r="B40" s="31"/>
       <c r="C40" s="7">
         <v>1</v>
       </c>
@@ -12971,10 +12948,10 @@
       </c>
     </row>
     <row r="41" spans="1:4" ht="12.75" customHeight="1">
-      <c r="A41" s="31" t="s">
+      <c r="A41" s="30" t="s">
         <v>491</v>
       </c>
-      <c r="B41" s="32"/>
+      <c r="B41" s="31"/>
       <c r="C41" s="7">
         <v>1</v>
       </c>
@@ -12983,10 +12960,10 @@
       </c>
     </row>
     <row r="42" spans="1:4" ht="12.75" customHeight="1">
-      <c r="A42" s="31" t="s">
+      <c r="A42" s="30" t="s">
         <v>2715</v>
       </c>
-      <c r="B42" s="32"/>
+      <c r="B42" s="31"/>
       <c r="C42" s="7">
         <v>1</v>
       </c>
@@ -12995,10 +12972,10 @@
       </c>
     </row>
     <row r="43" spans="1:4" ht="12.75" customHeight="1">
-      <c r="A43" s="31" t="s">
+      <c r="A43" s="30" t="s">
         <v>2569</v>
       </c>
-      <c r="B43" s="32"/>
+      <c r="B43" s="31"/>
       <c r="C43" s="7">
         <v>14</v>
       </c>
@@ -13007,10 +12984,10 @@
       </c>
     </row>
     <row r="44" spans="1:4" ht="12.75" customHeight="1">
-      <c r="A44" s="31" t="s">
+      <c r="A44" s="30" t="s">
         <v>3157</v>
       </c>
-      <c r="B44" s="32"/>
+      <c r="B44" s="31"/>
       <c r="C44" s="7">
         <v>1</v>
       </c>
@@ -13019,10 +12996,10 @@
       </c>
     </row>
     <row r="45" spans="1:4" ht="12.75" customHeight="1">
-      <c r="A45" s="31" t="s">
+      <c r="A45" s="30" t="s">
         <v>2665</v>
       </c>
-      <c r="B45" s="32"/>
+      <c r="B45" s="31"/>
       <c r="C45" s="7">
         <v>2</v>
       </c>
@@ -13031,10 +13008,10 @@
       </c>
     </row>
     <row r="46" spans="1:4" ht="12.75" customHeight="1">
-      <c r="A46" s="31" t="s">
+      <c r="A46" s="30" t="s">
         <v>2544</v>
       </c>
-      <c r="B46" s="32"/>
+      <c r="B46" s="31"/>
       <c r="C46" s="7">
         <v>2</v>
       </c>
@@ -13043,10 +13020,10 @@
       </c>
     </row>
     <row r="47" spans="1:4" ht="12.75" customHeight="1">
-      <c r="A47" s="31" t="s">
+      <c r="A47" s="30" t="s">
         <v>2791</v>
       </c>
-      <c r="B47" s="32"/>
+      <c r="B47" s="31"/>
       <c r="C47" s="7">
         <v>11</v>
       </c>
@@ -13055,10 +13032,10 @@
       </c>
     </row>
     <row r="48" spans="1:4" ht="12.75" customHeight="1">
-      <c r="A48" s="31" t="s">
+      <c r="A48" s="30" t="s">
         <v>2805</v>
       </c>
-      <c r="B48" s="32"/>
+      <c r="B48" s="31"/>
       <c r="C48" s="7">
         <v>4</v>
       </c>
@@ -13067,10 +13044,10 @@
       </c>
     </row>
     <row r="49" spans="1:4" ht="12.75" customHeight="1">
-      <c r="A49" s="31" t="s">
+      <c r="A49" s="30" t="s">
         <v>2776</v>
       </c>
-      <c r="B49" s="32"/>
+      <c r="B49" s="31"/>
       <c r="C49" s="7">
         <v>8</v>
       </c>
@@ -13079,10 +13056,10 @@
       </c>
     </row>
     <row r="50" spans="1:4" ht="12.75" customHeight="1">
-      <c r="A50" s="31" t="s">
+      <c r="A50" s="30" t="s">
         <v>3804</v>
       </c>
-      <c r="B50" s="32"/>
+      <c r="B50" s="31"/>
       <c r="C50" s="7">
         <v>1</v>
       </c>
@@ -13091,10 +13068,10 @@
       </c>
     </row>
     <row r="51" spans="1:4" ht="12.75" customHeight="1">
-      <c r="A51" s="31" t="s">
+      <c r="A51" s="30" t="s">
         <v>3805</v>
       </c>
-      <c r="B51" s="32"/>
+      <c r="B51" s="31"/>
       <c r="C51" s="7">
         <v>3</v>
       </c>
@@ -13103,10 +13080,10 @@
       </c>
     </row>
     <row r="52" spans="1:4" ht="12.75" customHeight="1">
-      <c r="A52" s="31" t="s">
+      <c r="A52" s="30" t="s">
         <v>3806</v>
       </c>
-      <c r="B52" s="32"/>
+      <c r="B52" s="31"/>
       <c r="C52" s="7">
         <v>1</v>
       </c>
@@ -13115,10 +13092,10 @@
       </c>
     </row>
     <row r="53" spans="1:4" ht="12.75" customHeight="1">
-      <c r="A53" s="31" t="s">
+      <c r="A53" s="30" t="s">
         <v>3323</v>
       </c>
-      <c r="B53" s="32"/>
+      <c r="B53" s="31"/>
       <c r="C53" s="7">
         <v>1</v>
       </c>
@@ -13127,10 +13104,10 @@
       </c>
     </row>
     <row r="54" spans="1:4" ht="12.75" customHeight="1">
-      <c r="A54" s="31" t="s">
+      <c r="A54" s="30" t="s">
         <v>2864</v>
       </c>
-      <c r="B54" s="32"/>
+      <c r="B54" s="31"/>
       <c r="C54" s="7">
         <v>4</v>
       </c>
@@ -13139,10 +13116,10 @@
       </c>
     </row>
     <row r="55" spans="1:4" ht="12.75" customHeight="1">
-      <c r="A55" s="31" t="s">
+      <c r="A55" s="30" t="s">
         <v>2778</v>
       </c>
-      <c r="B55" s="32"/>
+      <c r="B55" s="31"/>
       <c r="C55" s="7">
         <v>1</v>
       </c>
@@ -13151,10 +13128,10 @@
       </c>
     </row>
     <row r="56" spans="1:4" ht="12.75" customHeight="1">
-      <c r="A56" s="31" t="s">
+      <c r="A56" s="30" t="s">
         <v>2779</v>
       </c>
-      <c r="B56" s="32"/>
+      <c r="B56" s="31"/>
       <c r="C56" s="7">
         <v>1</v>
       </c>
@@ -13163,10 +13140,10 @@
       </c>
     </row>
     <row r="57" spans="1:4" ht="12.75" customHeight="1">
-      <c r="A57" s="31" t="s">
+      <c r="A57" s="30" t="s">
         <v>2780</v>
       </c>
-      <c r="B57" s="32"/>
+      <c r="B57" s="31"/>
       <c r="C57" s="7">
         <v>1</v>
       </c>
@@ -13175,10 +13152,10 @@
       </c>
     </row>
     <row r="58" spans="1:4" ht="12.75" customHeight="1">
-      <c r="A58" s="31" t="s">
+      <c r="A58" s="30" t="s">
         <v>2781</v>
       </c>
-      <c r="B58" s="32"/>
+      <c r="B58" s="31"/>
       <c r="C58" s="7">
         <v>8</v>
       </c>
@@ -13187,10 +13164,10 @@
       </c>
     </row>
     <row r="59" spans="1:4" ht="12.75" customHeight="1">
-      <c r="A59" s="31" t="s">
+      <c r="A59" s="30" t="s">
         <v>2792</v>
       </c>
-      <c r="B59" s="32"/>
+      <c r="B59" s="31"/>
       <c r="C59" s="7">
         <v>1</v>
       </c>
@@ -13199,10 +13176,10 @@
       </c>
     </row>
     <row r="60" spans="1:4" ht="12.75" customHeight="1">
-      <c r="A60" s="31" t="s">
+      <c r="A60" s="30" t="s">
         <v>2823</v>
       </c>
-      <c r="B60" s="32"/>
+      <c r="B60" s="31"/>
       <c r="C60" s="7">
         <v>1</v>
       </c>
@@ -13211,10 +13188,10 @@
       </c>
     </row>
     <row r="61" spans="1:4" ht="12.75" customHeight="1">
-      <c r="A61" s="31" t="s">
+      <c r="A61" s="30" t="s">
         <v>406</v>
       </c>
-      <c r="B61" s="32"/>
+      <c r="B61" s="31"/>
       <c r="C61" s="7">
         <v>3</v>
       </c>
@@ -13223,10 +13200,10 @@
       </c>
     </row>
     <row r="62" spans="1:4" ht="12.75" customHeight="1">
-      <c r="A62" s="31" t="s">
+      <c r="A62" s="30" t="s">
         <v>2551</v>
       </c>
-      <c r="B62" s="32"/>
+      <c r="B62" s="31"/>
       <c r="C62" s="7">
         <v>12</v>
       </c>
@@ -13235,10 +13212,10 @@
       </c>
     </row>
     <row r="63" spans="1:4" ht="12.75" customHeight="1">
-      <c r="A63" s="31" t="s">
+      <c r="A63" s="30" t="s">
         <v>3539</v>
       </c>
-      <c r="B63" s="32"/>
+      <c r="B63" s="31"/>
       <c r="C63" s="7">
         <v>1</v>
       </c>
@@ -13247,10 +13224,10 @@
       </c>
     </row>
     <row r="64" spans="1:4" ht="12.75" customHeight="1">
-      <c r="A64" s="31" t="s">
+      <c r="A64" s="30" t="s">
         <v>2667</v>
       </c>
-      <c r="B64" s="32"/>
+      <c r="B64" s="31"/>
       <c r="C64" s="7">
         <v>1</v>
       </c>
@@ -13259,10 +13236,10 @@
       </c>
     </row>
     <row r="65" spans="1:4" ht="12.75" customHeight="1">
-      <c r="A65" s="31" t="s">
+      <c r="A65" s="30" t="s">
         <v>2806</v>
       </c>
-      <c r="B65" s="32"/>
+      <c r="B65" s="31"/>
       <c r="C65" s="7">
         <v>1</v>
       </c>
@@ -13271,10 +13248,10 @@
       </c>
     </row>
     <row r="66" spans="1:4" ht="12.75" customHeight="1">
-      <c r="A66" s="31" t="s">
+      <c r="A66" s="30" t="s">
         <v>3540</v>
       </c>
-      <c r="B66" s="32"/>
+      <c r="B66" s="31"/>
       <c r="C66" s="7">
         <v>2</v>
       </c>
@@ -13283,10 +13260,10 @@
       </c>
     </row>
     <row r="67" spans="1:4" ht="12.75" customHeight="1">
-      <c r="A67" s="31" t="s">
+      <c r="A67" s="30" t="s">
         <v>2807</v>
       </c>
-      <c r="B67" s="32"/>
+      <c r="B67" s="31"/>
       <c r="C67" s="7">
         <v>3</v>
       </c>
@@ -13295,10 +13272,10 @@
       </c>
     </row>
     <row r="68" spans="1:4" ht="12.75" customHeight="1">
-      <c r="A68" s="31" t="s">
+      <c r="A68" s="30" t="s">
         <v>2808</v>
       </c>
-      <c r="B68" s="32"/>
+      <c r="B68" s="31"/>
       <c r="C68" s="7">
         <v>2</v>
       </c>
@@ -13307,10 +13284,10 @@
       </c>
     </row>
     <row r="69" spans="1:4" ht="12.75" customHeight="1">
-      <c r="A69" s="31" t="s">
+      <c r="A69" s="30" t="s">
         <v>2589</v>
       </c>
-      <c r="B69" s="32"/>
+      <c r="B69" s="31"/>
       <c r="C69" s="7">
         <v>4</v>
       </c>
@@ -13319,10 +13296,10 @@
       </c>
     </row>
     <row r="70" spans="1:4" ht="12.75" customHeight="1">
-      <c r="A70" s="31" t="s">
+      <c r="A70" s="30" t="s">
         <v>2574</v>
       </c>
-      <c r="B70" s="32"/>
+      <c r="B70" s="31"/>
       <c r="C70" s="7">
         <v>3</v>
       </c>
@@ -13331,10 +13308,10 @@
       </c>
     </row>
     <row r="71" spans="1:4" ht="12.75" customHeight="1">
-      <c r="A71" s="31" t="s">
+      <c r="A71" s="30" t="s">
         <v>2575</v>
       </c>
-      <c r="B71" s="32"/>
+      <c r="B71" s="31"/>
       <c r="C71" s="7">
         <v>4</v>
       </c>
@@ -13343,10 +13320,10 @@
       </c>
     </row>
     <row r="72" spans="1:4" ht="12.75" customHeight="1">
-      <c r="A72" s="31" t="s">
+      <c r="A72" s="30" t="s">
         <v>3325</v>
       </c>
-      <c r="B72" s="32"/>
+      <c r="B72" s="31"/>
       <c r="C72" s="7">
         <v>3</v>
       </c>
@@ -13355,10 +13332,10 @@
       </c>
     </row>
     <row r="73" spans="1:4" ht="12.75" customHeight="1">
-      <c r="A73" s="31" t="s">
+      <c r="A73" s="30" t="s">
         <v>3541</v>
       </c>
-      <c r="B73" s="32"/>
+      <c r="B73" s="31"/>
       <c r="C73" s="7">
         <v>1</v>
       </c>
@@ -13367,10 +13344,10 @@
       </c>
     </row>
     <row r="74" spans="1:4" ht="12.75" customHeight="1">
-      <c r="A74" s="31" t="s">
+      <c r="A74" s="30" t="s">
         <v>492</v>
       </c>
-      <c r="B74" s="32"/>
+      <c r="B74" s="31"/>
       <c r="C74" s="7">
         <v>2</v>
       </c>
@@ -13379,10 +13356,10 @@
       </c>
     </row>
     <row r="75" spans="1:4" ht="12.75" customHeight="1">
-      <c r="A75" s="31" t="s">
+      <c r="A75" s="30" t="s">
         <v>493</v>
       </c>
-      <c r="B75" s="32"/>
+      <c r="B75" s="31"/>
       <c r="C75" s="7">
         <v>5</v>
       </c>
@@ -13391,10 +13368,10 @@
       </c>
     </row>
     <row r="76" spans="1:4" ht="12.75" customHeight="1">
-      <c r="A76" s="31" t="s">
+      <c r="A76" s="30" t="s">
         <v>494</v>
       </c>
-      <c r="B76" s="32"/>
+      <c r="B76" s="31"/>
       <c r="C76" s="7">
         <v>5</v>
       </c>
@@ -13403,10 +13380,10 @@
       </c>
     </row>
     <row r="77" spans="1:4" ht="12.75" customHeight="1">
-      <c r="A77" s="31" t="s">
+      <c r="A77" s="30" t="s">
         <v>2825</v>
       </c>
-      <c r="B77" s="32"/>
+      <c r="B77" s="31"/>
       <c r="C77" s="7">
         <v>2</v>
       </c>
@@ -13415,10 +13392,10 @@
       </c>
     </row>
     <row r="78" spans="1:4" ht="12.75" customHeight="1">
-      <c r="A78" s="31" t="s">
+      <c r="A78" s="30" t="s">
         <v>2668</v>
       </c>
-      <c r="B78" s="32"/>
+      <c r="B78" s="31"/>
       <c r="C78" s="7">
         <v>1</v>
       </c>
@@ -13427,10 +13404,10 @@
       </c>
     </row>
     <row r="79" spans="1:4" ht="12.75" customHeight="1">
-      <c r="A79" s="31" t="s">
+      <c r="A79" s="30" t="s">
         <v>2669</v>
       </c>
-      <c r="B79" s="32"/>
+      <c r="B79" s="31"/>
       <c r="C79" s="7">
         <v>5</v>
       </c>
@@ -13439,10 +13416,10 @@
       </c>
     </row>
     <row r="80" spans="1:4" ht="12.75" customHeight="1">
-      <c r="A80" s="31" t="s">
+      <c r="A80" s="30" t="s">
         <v>495</v>
       </c>
-      <c r="B80" s="32"/>
+      <c r="B80" s="31"/>
       <c r="C80" s="7">
         <v>4</v>
       </c>
@@ -13451,10 +13428,10 @@
       </c>
     </row>
     <row r="81" spans="1:4" ht="12.75" customHeight="1">
-      <c r="A81" s="31" t="s">
+      <c r="A81" s="30" t="s">
         <v>3326</v>
       </c>
-      <c r="B81" s="32"/>
+      <c r="B81" s="31"/>
       <c r="C81" s="7">
         <v>2</v>
       </c>
@@ -13463,10 +13440,10 @@
       </c>
     </row>
     <row r="82" spans="1:4" ht="12.75" customHeight="1">
-      <c r="A82" s="31" t="s">
+      <c r="A82" s="30" t="s">
         <v>3807</v>
       </c>
-      <c r="B82" s="32"/>
+      <c r="B82" s="31"/>
       <c r="C82" s="7">
         <v>2</v>
       </c>
@@ -13475,10 +13452,10 @@
       </c>
     </row>
     <row r="83" spans="1:4" ht="12.75" customHeight="1">
-      <c r="A83" s="31" t="s">
+      <c r="A83" s="30" t="s">
         <v>2793</v>
       </c>
-      <c r="B83" s="32"/>
+      <c r="B83" s="31"/>
       <c r="C83" s="7">
         <v>1</v>
       </c>
@@ -13487,10 +13464,10 @@
       </c>
     </row>
     <row r="84" spans="1:4" ht="12.75" customHeight="1">
-      <c r="A84" s="31" t="s">
+      <c r="A84" s="30" t="s">
         <v>3041</v>
       </c>
-      <c r="B84" s="32"/>
+      <c r="B84" s="31"/>
       <c r="C84" s="7">
         <v>1</v>
       </c>
@@ -13499,10 +13476,10 @@
       </c>
     </row>
     <row r="85" spans="1:4" ht="12.75" customHeight="1">
-      <c r="A85" s="31" t="s">
+      <c r="A85" s="30" t="s">
         <v>3042</v>
       </c>
-      <c r="B85" s="32"/>
+      <c r="B85" s="31"/>
       <c r="C85" s="7">
         <v>5</v>
       </c>
@@ -13511,10 +13488,10 @@
       </c>
     </row>
     <row r="86" spans="1:4" ht="12.75" customHeight="1">
-      <c r="A86" s="31" t="s">
+      <c r="A86" s="30" t="s">
         <v>2570</v>
       </c>
-      <c r="B86" s="32"/>
+      <c r="B86" s="31"/>
       <c r="C86" s="7">
         <v>3</v>
       </c>
@@ -13523,10 +13500,10 @@
       </c>
     </row>
     <row r="87" spans="1:4" ht="12.75" customHeight="1">
-      <c r="A87" s="31" t="s">
+      <c r="A87" s="30" t="s">
         <v>2571</v>
       </c>
-      <c r="B87" s="32"/>
+      <c r="B87" s="31"/>
       <c r="C87" s="7">
         <v>4</v>
       </c>
@@ -13535,10 +13512,10 @@
       </c>
     </row>
     <row r="88" spans="1:4" ht="12.75" customHeight="1">
-      <c r="A88" s="31" t="s">
+      <c r="A88" s="30" t="s">
         <v>3542</v>
       </c>
-      <c r="B88" s="32"/>
+      <c r="B88" s="31"/>
       <c r="C88" s="7">
         <v>1</v>
       </c>
@@ -13547,10 +13524,10 @@
       </c>
     </row>
     <row r="89" spans="1:4" ht="12.75" customHeight="1">
-      <c r="A89" s="31" t="s">
+      <c r="A89" s="30" t="s">
         <v>3543</v>
       </c>
-      <c r="B89" s="32"/>
+      <c r="B89" s="31"/>
       <c r="C89" s="7">
         <v>1</v>
       </c>
@@ -13559,14 +13536,14 @@
       </c>
     </row>
     <row r="90" spans="1:4" ht="12.75" customHeight="1">
-      <c r="A90" s="30"/>
-      <c r="B90" s="30"/>
+      <c r="A90" s="29"/>
+      <c r="B90" s="29"/>
     </row>
     <row r="91" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A91" s="33" t="s">
+      <c r="A91" s="32" t="s">
         <v>272</v>
       </c>
-      <c r="B91" s="33"/>
+      <c r="B91" s="32"/>
     </row>
     <row r="92" spans="1:4" ht="14.25" customHeight="1">
       <c r="A92" s="27" t="s">
@@ -14677,19 +14654,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="33" t="s">
         <v>107</v>
       </c>
-      <c r="B1" s="29"/>
-      <c r="C1" s="29"/>
+      <c r="B1" s="33"/>
+      <c r="C1" s="33"/>
     </row>
     <row r="2" spans="1:3">
-      <c r="A2" s="29" t="str">
+      <c r="A2" s="33" t="str">
         <f ca="1">"TANGGAL : "&amp;SUBSTITUTE(MID(CELL("filename"),SEARCH("[",CELL("filename"))+1, SEARCH("]",CELL("filename"))-SEARCH("[",CELL("filename"))-1),".xlsx","")</f>
         <v>TANGGAL : 23 SEPTEMBER - 28 SEPTEMBER</v>
       </c>
-      <c r="B2" s="29"/>
-      <c r="C2" s="29"/>
+      <c r="B2" s="33"/>
+      <c r="C2" s="33"/>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="10" t="s">
@@ -37905,10 +37882,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E95"/>
+  <dimension ref="A1:D95"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A80" zoomScale="70" zoomScaleNormal="130" zoomScaleSheetLayoutView="85" zoomScalePageLayoutView="70" workbookViewId="0">
-      <selection activeCell="B91" sqref="B91"/>
+    <sheetView view="pageLayout" topLeftCell="A74" zoomScale="70" zoomScaleNormal="130" zoomScaleSheetLayoutView="85" zoomScalePageLayoutView="70" workbookViewId="0">
+      <selection activeCell="A107" sqref="A107"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -38172,7 +38149,7 @@
     <col min="16128" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="25" customFormat="1" ht="15">
+    <row r="1" spans="1:4" s="25" customFormat="1" ht="15">
       <c r="A1" s="22" t="s">
         <v>3613</v>
       </c>
@@ -38180,7 +38157,7 @@
       <c r="C1" s="23"/>
       <c r="D1" s="24"/>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:4">
       <c r="A2" s="18" t="s">
         <v>3614</v>
       </c>
@@ -38193,11 +38170,8 @@
       <c r="D2" s="21" t="s">
         <v>542</v>
       </c>
-      <c r="E2" s="2" t="s">
-        <v>3832</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
+    </row>
+    <row r="3" spans="1:4">
       <c r="A3" s="18" t="s">
         <v>3616</v>
       </c>
@@ -38210,11 +38184,8 @@
       <c r="D3" s="21" t="s">
         <v>115</v>
       </c>
-      <c r="E3" s="2" t="s">
-        <v>3832</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
+    </row>
+    <row r="4" spans="1:4">
       <c r="A4" s="18" t="s">
         <v>3618</v>
       </c>
@@ -38227,11 +38198,8 @@
       <c r="D4" s="21" t="s">
         <v>119</v>
       </c>
-      <c r="E4" s="2" t="s">
-        <v>3832</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
+    </row>
+    <row r="5" spans="1:4">
       <c r="A5" s="18" t="s">
         <v>3620</v>
       </c>
@@ -38244,11 +38212,8 @@
       <c r="D5" s="21" t="s">
         <v>536</v>
       </c>
-      <c r="E5" s="2" t="s">
-        <v>3832</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5">
+    </row>
+    <row r="6" spans="1:4">
       <c r="A6" s="18" t="s">
         <v>3622</v>
       </c>
@@ -38261,11 +38226,8 @@
       <c r="D6" s="21" t="s">
         <v>536</v>
       </c>
-      <c r="E6" s="2" t="s">
-        <v>3832</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5">
+    </row>
+    <row r="7" spans="1:4">
       <c r="A7" s="18" t="s">
         <v>3624</v>
       </c>
@@ -38278,11 +38240,8 @@
       <c r="D7" s="21" t="s">
         <v>119</v>
       </c>
-      <c r="E7" s="2" t="s">
-        <v>2543</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5">
+    </row>
+    <row r="8" spans="1:4">
       <c r="A8" s="18" t="s">
         <v>3626</v>
       </c>
@@ -38295,11 +38254,8 @@
       <c r="D8" s="21" t="s">
         <v>429</v>
       </c>
-      <c r="E8" s="2" t="s">
-        <v>2543</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5">
+    </row>
+    <row r="9" spans="1:4">
       <c r="A9" s="18" t="s">
         <v>3628</v>
       </c>
@@ -38312,11 +38268,8 @@
       <c r="D9" s="21" t="s">
         <v>148</v>
       </c>
-      <c r="E9" s="2" t="s">
-        <v>3832</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5">
+    </row>
+    <row r="10" spans="1:4">
       <c r="A10" s="18" t="s">
         <v>3630</v>
       </c>
@@ -38329,11 +38282,8 @@
       <c r="D10" s="21" t="s">
         <v>536</v>
       </c>
-      <c r="E10" s="2" t="s">
-        <v>3832</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5">
+    </row>
+    <row r="11" spans="1:4">
       <c r="A11" s="18" t="s">
         <v>3632</v>
       </c>
@@ -38346,11 +38296,8 @@
       <c r="D11" s="21" t="s">
         <v>256</v>
       </c>
-      <c r="E11" s="2" t="s">
-        <v>3832</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5">
+    </row>
+    <row r="12" spans="1:4">
       <c r="A12" s="18" t="s">
         <v>3634</v>
       </c>
@@ -38363,11 +38310,8 @@
       <c r="D12" s="21" t="s">
         <v>119</v>
       </c>
-      <c r="E12" s="2" t="s">
-        <v>3832</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5">
+    </row>
+    <row r="13" spans="1:4">
       <c r="A13" s="18" t="s">
         <v>3636</v>
       </c>
@@ -38380,11 +38324,8 @@
       <c r="D13" s="21" t="s">
         <v>3638</v>
       </c>
-      <c r="E13" s="2" t="s">
-        <v>2543</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5">
+    </row>
+    <row r="14" spans="1:4">
       <c r="A14" s="18" t="s">
         <v>3639</v>
       </c>
@@ -38397,11 +38338,8 @@
       <c r="D14" s="21" t="s">
         <v>119</v>
       </c>
-      <c r="E14" s="2" t="s">
-        <v>3832</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5">
+    </row>
+    <row r="15" spans="1:4">
       <c r="A15" s="18" t="s">
         <v>3641</v>
       </c>
@@ -38414,11 +38352,8 @@
       <c r="D15" s="21" t="s">
         <v>429</v>
       </c>
-      <c r="E15" s="2" t="s">
-        <v>3832</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5">
+    </row>
+    <row r="16" spans="1:4">
       <c r="A16" s="18" t="s">
         <v>3643</v>
       </c>
@@ -38431,11 +38366,8 @@
       <c r="D16" s="21" t="s">
         <v>109</v>
       </c>
-      <c r="E16" s="2" t="s">
-        <v>3832</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5">
+    </row>
+    <row r="17" spans="1:4">
       <c r="A17" s="18" t="s">
         <v>3645</v>
       </c>
@@ -38448,11 +38380,8 @@
       <c r="D17" s="21" t="s">
         <v>119</v>
       </c>
-      <c r="E17" s="2" t="s">
-        <v>3832</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5">
+    </row>
+    <row r="18" spans="1:4">
       <c r="A18" s="18" t="s">
         <v>3647</v>
       </c>
@@ -38465,11 +38394,8 @@
       <c r="D18" s="21" t="s">
         <v>392</v>
       </c>
-      <c r="E18" s="2" t="s">
-        <v>3832</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5">
+    </row>
+    <row r="19" spans="1:4">
       <c r="A19" s="18" t="s">
         <v>3649</v>
       </c>
@@ -38482,11 +38408,8 @@
       <c r="D19" s="21" t="s">
         <v>131</v>
       </c>
-      <c r="E19" s="2" t="s">
-        <v>3832</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5">
+    </row>
+    <row r="20" spans="1:4">
       <c r="A20" s="18" t="s">
         <v>3651</v>
       </c>
@@ -38499,11 +38422,8 @@
       <c r="D20" s="21" t="s">
         <v>148</v>
       </c>
-      <c r="E20" s="2" t="s">
-        <v>3832</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5">
+    </row>
+    <row r="21" spans="1:4">
       <c r="A21" s="18" t="s">
         <v>3653</v>
       </c>
@@ -38516,11 +38436,8 @@
       <c r="D21" s="21" t="s">
         <v>3655</v>
       </c>
-      <c r="E21" s="2" t="s">
-        <v>2543</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5">
+    </row>
+    <row r="22" spans="1:4">
       <c r="A22" s="18" t="s">
         <v>3656</v>
       </c>
@@ -38533,11 +38450,8 @@
       <c r="D22" s="21" t="s">
         <v>536</v>
       </c>
-      <c r="E22" s="2" t="s">
-        <v>3832</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5">
+    </row>
+    <row r="23" spans="1:4">
       <c r="A23" s="18" t="s">
         <v>3658</v>
       </c>
@@ -38550,11 +38464,8 @@
       <c r="D23" s="21" t="s">
         <v>119</v>
       </c>
-      <c r="E23" s="2" t="s">
-        <v>3832</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5">
+    </row>
+    <row r="24" spans="1:4">
       <c r="A24" s="18" t="s">
         <v>3660</v>
       </c>
@@ -38567,11 +38478,8 @@
       <c r="D24" s="21" t="s">
         <v>418</v>
       </c>
-      <c r="E24" s="2" t="s">
-        <v>3832</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5">
+    </row>
+    <row r="25" spans="1:4">
       <c r="A25" s="18" t="s">
         <v>3662</v>
       </c>
@@ -38584,11 +38492,8 @@
       <c r="D25" s="21" t="s">
         <v>545</v>
       </c>
-      <c r="E25" s="2" t="s">
-        <v>3832</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5">
+    </row>
+    <row r="26" spans="1:4">
       <c r="A26" s="18" t="s">
         <v>3664</v>
       </c>
@@ -38601,11 +38506,8 @@
       <c r="D26" s="21" t="s">
         <v>464</v>
       </c>
-      <c r="E26" s="2" t="s">
-        <v>3832</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5">
+    </row>
+    <row r="27" spans="1:4">
       <c r="A27" s="18" t="s">
         <v>3666</v>
       </c>
@@ -38618,11 +38520,8 @@
       <c r="D27" s="21" t="s">
         <v>110</v>
       </c>
-      <c r="E27" s="2" t="s">
-        <v>3832</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5">
+    </row>
+    <row r="28" spans="1:4">
       <c r="A28" s="18" t="s">
         <v>3668</v>
       </c>
@@ -38635,11 +38534,8 @@
       <c r="D28" s="21" t="s">
         <v>110</v>
       </c>
-      <c r="E28" s="2" t="s">
-        <v>3832</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5">
+    </row>
+    <row r="29" spans="1:4">
       <c r="A29" s="18" t="s">
         <v>1</v>
       </c>
@@ -38652,11 +38548,8 @@
       <c r="D29" s="21" t="s">
         <v>139</v>
       </c>
-      <c r="E29" s="2" t="s">
-        <v>3832</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5">
+    </row>
+    <row r="30" spans="1:4">
       <c r="A30" s="18" t="s">
         <v>3671</v>
       </c>
@@ -38669,11 +38562,8 @@
       <c r="D30" s="21" t="s">
         <v>110</v>
       </c>
-      <c r="E30" s="2" t="s">
-        <v>3832</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5">
+    </row>
+    <row r="31" spans="1:4">
       <c r="A31" s="18" t="s">
         <v>3673</v>
       </c>
@@ -38686,11 +38576,8 @@
       <c r="D31" s="21" t="s">
         <v>547</v>
       </c>
-      <c r="E31" s="2" t="s">
-        <v>3832</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5">
+    </row>
+    <row r="32" spans="1:4">
       <c r="A32" s="18" t="s">
         <v>3675</v>
       </c>
@@ -38703,11 +38590,8 @@
       <c r="D32" s="21" t="s">
         <v>128</v>
       </c>
-      <c r="E32" s="2" t="s">
-        <v>2543</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5">
+    </row>
+    <row r="33" spans="1:4">
       <c r="A33" s="18" t="s">
         <v>3677</v>
       </c>
@@ -38720,11 +38604,8 @@
       <c r="D33" s="21" t="s">
         <v>128</v>
       </c>
-      <c r="E33" s="2" t="s">
-        <v>2543</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5">
+    </row>
+    <row r="34" spans="1:4">
       <c r="A34" s="18" t="s">
         <v>3679</v>
       </c>
@@ -38737,11 +38618,8 @@
       <c r="D34" s="21" t="s">
         <v>128</v>
       </c>
-      <c r="E34" s="2" t="s">
-        <v>2543</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5">
+    </row>
+    <row r="35" spans="1:4">
       <c r="A35" s="18" t="s">
         <v>3681</v>
       </c>
@@ -38754,11 +38632,8 @@
       <c r="D35" s="21" t="s">
         <v>128</v>
       </c>
-      <c r="E35" s="2" t="s">
-        <v>2543</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5">
+    </row>
+    <row r="36" spans="1:4">
       <c r="A36" s="18" t="s">
         <v>3683</v>
       </c>
@@ -38771,11 +38646,8 @@
       <c r="D36" s="21" t="s">
         <v>128</v>
       </c>
-      <c r="E36" s="2" t="s">
-        <v>2543</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5">
+    </row>
+    <row r="37" spans="1:4">
       <c r="A37" s="18" t="s">
         <v>3685</v>
       </c>
@@ -38788,11 +38660,8 @@
       <c r="D37" s="21" t="s">
         <v>128</v>
       </c>
-      <c r="E37" s="2" t="s">
-        <v>2543</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5">
+    </row>
+    <row r="38" spans="1:4">
       <c r="A38" s="18" t="s">
         <v>3687</v>
       </c>
@@ -38805,11 +38674,8 @@
       <c r="D38" s="21" t="s">
         <v>159</v>
       </c>
-      <c r="E38" s="2" t="s">
-        <v>2543</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5">
+    </row>
+    <row r="39" spans="1:4">
       <c r="A39" s="18" t="s">
         <v>3689</v>
       </c>
@@ -38822,11 +38688,8 @@
       <c r="D39" s="21" t="s">
         <v>128</v>
       </c>
-      <c r="E39" s="2" t="s">
-        <v>3832</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5">
+    </row>
+    <row r="40" spans="1:4">
       <c r="A40" s="18" t="s">
         <v>3691</v>
       </c>
@@ -38839,11 +38702,8 @@
       <c r="D40" s="21" t="s">
         <v>128</v>
       </c>
-      <c r="E40" s="2" t="s">
-        <v>2543</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5">
+    </row>
+    <row r="41" spans="1:4">
       <c r="A41" s="18" t="s">
         <v>3693</v>
       </c>
@@ -38856,11 +38716,8 @@
       <c r="D41" s="21" t="s">
         <v>124</v>
       </c>
-      <c r="E41" s="2" t="s">
-        <v>3832</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5">
+    </row>
+    <row r="42" spans="1:4">
       <c r="A42" s="18" t="s">
         <v>3695</v>
       </c>
@@ -38873,11 +38730,8 @@
       <c r="D42" s="21" t="s">
         <v>137</v>
       </c>
-      <c r="E42" s="2" t="s">
-        <v>2543</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5">
+    </row>
+    <row r="43" spans="1:4">
       <c r="A43" s="18" t="s">
         <v>3697</v>
       </c>
@@ -38890,11 +38744,8 @@
       <c r="D43" s="21" t="s">
         <v>137</v>
       </c>
-      <c r="E43" s="2" t="s">
-        <v>2543</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5">
+    </row>
+    <row r="44" spans="1:4">
       <c r="A44" s="18" t="s">
         <v>2</v>
       </c>
@@ -38907,11 +38758,8 @@
       <c r="D44" s="21" t="s">
         <v>128</v>
       </c>
-      <c r="E44" s="2" t="s">
-        <v>3832</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5">
+    </row>
+    <row r="45" spans="1:4">
       <c r="A45" s="18" t="s">
         <v>3700</v>
       </c>
@@ -38924,11 +38772,8 @@
       <c r="D45" s="21" t="s">
         <v>128</v>
       </c>
-      <c r="E45" s="2" t="s">
-        <v>3832</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5">
+    </row>
+    <row r="46" spans="1:4">
       <c r="A46" s="18" t="s">
         <v>132</v>
       </c>
@@ -38941,11 +38786,8 @@
       <c r="D46" s="21" t="s">
         <v>110</v>
       </c>
-      <c r="E46" s="2" t="s">
-        <v>3832</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5">
+    </row>
+    <row r="47" spans="1:4">
       <c r="A47" s="18" t="s">
         <v>3703</v>
       </c>
@@ -38958,11 +38800,8 @@
       <c r="D47" s="21" t="s">
         <v>110</v>
       </c>
-      <c r="E47" s="2" t="s">
-        <v>3832</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5">
+    </row>
+    <row r="48" spans="1:4">
       <c r="A48" s="18" t="s">
         <v>3705</v>
       </c>
@@ -38975,11 +38814,8 @@
       <c r="D48" s="21" t="s">
         <v>110</v>
       </c>
-      <c r="E48" s="2" t="s">
-        <v>2543</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5">
+    </row>
+    <row r="49" spans="1:4">
       <c r="A49" s="18" t="s">
         <v>3707</v>
       </c>
@@ -38992,11 +38828,8 @@
       <c r="D49" s="21" t="s">
         <v>159</v>
       </c>
-      <c r="E49" s="2" t="s">
-        <v>2543</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5">
+    </row>
+    <row r="50" spans="1:4">
       <c r="A50" s="18" t="s">
         <v>3709</v>
       </c>
@@ -39009,11 +38842,8 @@
       <c r="D50" s="21" t="s">
         <v>128</v>
       </c>
-      <c r="E50" s="2" t="s">
-        <v>3832</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5">
+    </row>
+    <row r="51" spans="1:4">
       <c r="A51" s="18" t="s">
         <v>3711</v>
       </c>
@@ -39026,11 +38856,8 @@
       <c r="D51" s="21" t="s">
         <v>128</v>
       </c>
-      <c r="E51" s="2" t="s">
-        <v>2543</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5">
+    </row>
+    <row r="52" spans="1:4">
       <c r="A52" s="18" t="s">
         <v>3713</v>
       </c>
@@ -39043,11 +38870,8 @@
       <c r="D52" s="21" t="s">
         <v>137</v>
       </c>
-      <c r="E52" s="2" t="s">
-        <v>2543</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5">
+    </row>
+    <row r="53" spans="1:4">
       <c r="A53" s="18" t="s">
         <v>3715</v>
       </c>
@@ -39060,11 +38884,8 @@
       <c r="D53" s="21" t="s">
         <v>137</v>
       </c>
-      <c r="E53" s="2" t="s">
-        <v>2543</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5">
+    </row>
+    <row r="54" spans="1:4">
       <c r="A54" s="18" t="s">
         <v>3717</v>
       </c>
@@ -39077,11 +38898,8 @@
       <c r="D54" s="21" t="s">
         <v>137</v>
       </c>
-      <c r="E54" s="2" t="s">
-        <v>2543</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5">
+    </row>
+    <row r="55" spans="1:4">
       <c r="A55" s="18" t="s">
         <v>3719</v>
       </c>
@@ -39094,11 +38912,8 @@
       <c r="D55" s="21" t="s">
         <v>137</v>
       </c>
-      <c r="E55" s="2" t="s">
-        <v>3832</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5">
+    </row>
+    <row r="56" spans="1:4">
       <c r="A56" s="18" t="s">
         <v>1666</v>
       </c>
@@ -39111,11 +38926,8 @@
       <c r="D56" s="21" t="s">
         <v>137</v>
       </c>
-      <c r="E56" s="2" t="s">
-        <v>3832</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5">
+    </row>
+    <row r="57" spans="1:4">
       <c r="A57" s="18" t="s">
         <v>548</v>
       </c>
@@ -39128,11 +38940,8 @@
       <c r="D57" s="21" t="s">
         <v>156</v>
       </c>
-      <c r="E57" s="2" t="s">
-        <v>3832</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5">
+    </row>
+    <row r="58" spans="1:4">
       <c r="A58" s="18" t="s">
         <v>549</v>
       </c>
@@ -39145,11 +38954,8 @@
       <c r="D58" s="21" t="s">
         <v>550</v>
       </c>
-      <c r="E58" s="2" t="s">
-        <v>3832</v>
-      </c>
-    </row>
-    <row r="59" spans="1:5">
+    </row>
+    <row r="59" spans="1:4">
       <c r="A59" s="18" t="s">
         <v>3722</v>
       </c>
@@ -39162,11 +38968,8 @@
       <c r="D59" s="21" t="s">
         <v>542</v>
       </c>
-      <c r="E59" s="2" t="s">
-        <v>3832</v>
-      </c>
-    </row>
-    <row r="60" spans="1:5">
+    </row>
+    <row r="60" spans="1:4">
       <c r="A60" s="18" t="s">
         <v>3724</v>
       </c>
@@ -39179,11 +38982,8 @@
       <c r="D60" s="21" t="s">
         <v>518</v>
       </c>
-      <c r="E60" s="2" t="s">
-        <v>3832</v>
-      </c>
-    </row>
-    <row r="61" spans="1:5">
+    </row>
+    <row r="61" spans="1:4">
       <c r="A61" s="18" t="s">
         <v>3726</v>
       </c>
@@ -39196,11 +38996,8 @@
       <c r="D61" s="21" t="s">
         <v>3728</v>
       </c>
-      <c r="E61" s="2" t="s">
-        <v>2543</v>
-      </c>
-    </row>
-    <row r="62" spans="1:5">
+    </row>
+    <row r="62" spans="1:4">
       <c r="A62" s="18" t="s">
         <v>3729</v>
       </c>
@@ -39213,11 +39010,8 @@
       <c r="D62" s="21" t="s">
         <v>3731</v>
       </c>
-      <c r="E62" s="2" t="s">
-        <v>3832</v>
-      </c>
-    </row>
-    <row r="63" spans="1:5">
+    </row>
+    <row r="63" spans="1:4">
       <c r="A63" s="18" t="s">
         <v>3732</v>
       </c>
@@ -39230,11 +39024,8 @@
       <c r="D63" s="21" t="s">
         <v>3734</v>
       </c>
-      <c r="E63" s="2" t="s">
-        <v>2543</v>
-      </c>
-    </row>
-    <row r="64" spans="1:5">
+    </row>
+    <row r="64" spans="1:4">
       <c r="A64" s="18" t="s">
         <v>3735</v>
       </c>
@@ -39247,11 +39038,8 @@
       <c r="D64" s="21" t="s">
         <v>3737</v>
       </c>
-      <c r="E64" s="2" t="s">
-        <v>2543</v>
-      </c>
-    </row>
-    <row r="65" spans="1:5">
+    </row>
+    <row r="65" spans="1:4">
       <c r="A65" s="18" t="s">
         <v>3738</v>
       </c>
@@ -39264,11 +39052,8 @@
       <c r="D65" s="21" t="s">
         <v>3737</v>
       </c>
-      <c r="E65" s="2" t="s">
-        <v>2543</v>
-      </c>
-    </row>
-    <row r="66" spans="1:5">
+    </row>
+    <row r="66" spans="1:4">
       <c r="A66" s="18" t="s">
         <v>3740</v>
       </c>
@@ -39281,11 +39066,8 @@
       <c r="D66" s="21" t="s">
         <v>3737</v>
       </c>
-      <c r="E66" s="2" t="s">
-        <v>2543</v>
-      </c>
-    </row>
-    <row r="67" spans="1:5">
+    </row>
+    <row r="67" spans="1:4">
       <c r="A67" s="18" t="s">
         <v>3742</v>
       </c>
@@ -39298,11 +39080,8 @@
       <c r="D67" s="21" t="s">
         <v>3737</v>
       </c>
-      <c r="E67" s="2" t="s">
-        <v>2543</v>
-      </c>
-    </row>
-    <row r="68" spans="1:5">
+    </row>
+    <row r="68" spans="1:4">
       <c r="A68" s="18" t="s">
         <v>3744</v>
       </c>
@@ -39315,11 +39094,8 @@
       <c r="D68" s="21" t="s">
         <v>3737</v>
       </c>
-      <c r="E68" s="2" t="s">
-        <v>2543</v>
-      </c>
-    </row>
-    <row r="69" spans="1:5">
+    </row>
+    <row r="69" spans="1:4">
       <c r="A69" s="18" t="s">
         <v>3746</v>
       </c>
@@ -39332,11 +39108,8 @@
       <c r="D69" s="21" t="s">
         <v>3737</v>
       </c>
-      <c r="E69" s="2" t="s">
-        <v>2543</v>
-      </c>
-    </row>
-    <row r="70" spans="1:5">
+    </row>
+    <row r="70" spans="1:4">
       <c r="A70" s="18" t="s">
         <v>3748</v>
       </c>
@@ -39349,11 +39122,8 @@
       <c r="D70" s="21" t="s">
         <v>3737</v>
       </c>
-      <c r="E70" s="2" t="s">
-        <v>2543</v>
-      </c>
-    </row>
-    <row r="71" spans="1:5">
+    </row>
+    <row r="71" spans="1:4">
       <c r="A71" s="18" t="s">
         <v>3750</v>
       </c>
@@ -39366,11 +39136,8 @@
       <c r="D71" s="21" t="s">
         <v>148</v>
       </c>
-      <c r="E71" s="2" t="s">
-        <v>3832</v>
-      </c>
-    </row>
-    <row r="72" spans="1:5">
+    </row>
+    <row r="72" spans="1:4">
       <c r="A72" s="18" t="s">
         <v>3752</v>
       </c>
@@ -39383,11 +39150,8 @@
       <c r="D72" s="21" t="s">
         <v>148</v>
       </c>
-      <c r="E72" s="2" t="s">
-        <v>3832</v>
-      </c>
-    </row>
-    <row r="73" spans="1:5">
+    </row>
+    <row r="73" spans="1:4">
       <c r="A73" s="18" t="s">
         <v>3754</v>
       </c>
@@ -39400,11 +39164,8 @@
       <c r="D73" s="21" t="s">
         <v>3737</v>
       </c>
-      <c r="E73" s="2" t="s">
-        <v>2543</v>
-      </c>
-    </row>
-    <row r="74" spans="1:5">
+    </row>
+    <row r="74" spans="1:4">
       <c r="A74" s="18" t="s">
         <v>3756</v>
       </c>
@@ -39417,11 +39178,8 @@
       <c r="D74" s="21" t="s">
         <v>3758</v>
       </c>
-      <c r="E74" s="2" t="s">
-        <v>2543</v>
-      </c>
-    </row>
-    <row r="75" spans="1:5">
+    </row>
+    <row r="75" spans="1:4">
       <c r="A75" s="18" t="s">
         <v>3759</v>
       </c>
@@ -39434,11 +39192,8 @@
       <c r="D75" s="21" t="s">
         <v>3761</v>
       </c>
-      <c r="E75" s="2" t="s">
-        <v>3832</v>
-      </c>
-    </row>
-    <row r="76" spans="1:5">
+    </row>
+    <row r="76" spans="1:4">
       <c r="A76" s="18" t="s">
         <v>3048</v>
       </c>
@@ -39451,11 +39206,8 @@
       <c r="D76" s="21" t="s">
         <v>3049</v>
       </c>
-      <c r="E76" s="2" t="s">
-        <v>3832</v>
-      </c>
-    </row>
-    <row r="77" spans="1:5">
+    </row>
+    <row r="77" spans="1:4">
       <c r="A77" s="18" t="s">
         <v>3763</v>
       </c>
@@ -39468,11 +39220,8 @@
       <c r="D77" s="21" t="s">
         <v>3734</v>
       </c>
-      <c r="E77" s="2" t="s">
-        <v>3832</v>
-      </c>
-    </row>
-    <row r="78" spans="1:5">
+    </row>
+    <row r="78" spans="1:4">
       <c r="A78" s="18" t="s">
         <v>3765</v>
       </c>
@@ -39485,11 +39234,8 @@
       <c r="D78" s="21" t="s">
         <v>3737</v>
       </c>
-      <c r="E78" s="2" t="s">
-        <v>2543</v>
-      </c>
-    </row>
-    <row r="79" spans="1:5">
+    </row>
+    <row r="79" spans="1:4">
       <c r="A79" s="18" t="s">
         <v>3767</v>
       </c>
@@ -39502,11 +39248,8 @@
       <c r="D79" s="21" t="s">
         <v>160</v>
       </c>
-      <c r="E79" s="2" t="s">
-        <v>3832</v>
-      </c>
-    </row>
-    <row r="80" spans="1:5">
+    </row>
+    <row r="80" spans="1:4">
       <c r="A80" s="18" t="s">
         <v>3769</v>
       </c>
@@ -39519,11 +39262,8 @@
       <c r="D80" s="21" t="s">
         <v>160</v>
       </c>
-      <c r="E80" s="2" t="s">
-        <v>3832</v>
-      </c>
-    </row>
-    <row r="81" spans="1:5">
+    </row>
+    <row r="81" spans="1:4">
       <c r="A81" s="18" t="s">
         <v>3771</v>
       </c>
@@ -39536,11 +39276,8 @@
       <c r="D81" s="21" t="s">
         <v>160</v>
       </c>
-      <c r="E81" s="2" t="s">
-        <v>3832</v>
-      </c>
-    </row>
-    <row r="82" spans="1:5">
+    </row>
+    <row r="82" spans="1:4">
       <c r="A82" s="18" t="s">
         <v>3773</v>
       </c>
@@ -39553,11 +39290,8 @@
       <c r="D82" s="21" t="s">
         <v>160</v>
       </c>
-      <c r="E82" s="2" t="s">
-        <v>3832</v>
-      </c>
-    </row>
-    <row r="83" spans="1:5">
+    </row>
+    <row r="83" spans="1:4">
       <c r="A83" s="18" t="s">
         <v>3775</v>
       </c>
@@ -39570,11 +39304,8 @@
       <c r="D83" s="21" t="s">
         <v>160</v>
       </c>
-      <c r="E83" s="2" t="s">
-        <v>3832</v>
-      </c>
-    </row>
-    <row r="84" spans="1:5">
+    </row>
+    <row r="84" spans="1:4">
       <c r="A84" s="18" t="s">
         <v>3777</v>
       </c>
@@ -39587,11 +39318,8 @@
       <c r="D84" s="21" t="s">
         <v>160</v>
       </c>
-      <c r="E84" s="2" t="s">
-        <v>3832</v>
-      </c>
-    </row>
-    <row r="85" spans="1:5">
+    </row>
+    <row r="85" spans="1:4">
       <c r="A85" s="18" t="s">
         <v>3779</v>
       </c>
@@ -39604,11 +39332,8 @@
       <c r="D85" s="21" t="s">
         <v>160</v>
       </c>
-      <c r="E85" s="2" t="s">
-        <v>3832</v>
-      </c>
-    </row>
-    <row r="86" spans="1:5">
+    </row>
+    <row r="86" spans="1:4">
       <c r="A86" s="18" t="s">
         <v>3781</v>
       </c>
@@ -39621,11 +39346,8 @@
       <c r="D86" s="21" t="s">
         <v>160</v>
       </c>
-      <c r="E86" s="2" t="s">
-        <v>3832</v>
-      </c>
-    </row>
-    <row r="87" spans="1:5">
+    </row>
+    <row r="87" spans="1:4">
       <c r="A87" s="18" t="s">
         <v>3783</v>
       </c>
@@ -39638,11 +39360,8 @@
       <c r="D87" s="21" t="s">
         <v>160</v>
       </c>
-      <c r="E87" s="2" t="s">
-        <v>3832</v>
-      </c>
-    </row>
-    <row r="88" spans="1:5">
+    </row>
+    <row r="88" spans="1:4">
       <c r="A88" s="18" t="s">
         <v>3785</v>
       </c>
@@ -39655,11 +39374,8 @@
       <c r="D88" s="21" t="s">
         <v>3787</v>
       </c>
-      <c r="E88" s="2" t="s">
-        <v>3832</v>
-      </c>
-    </row>
-    <row r="89" spans="1:5">
+    </row>
+    <row r="89" spans="1:4">
       <c r="A89" s="18" t="s">
         <v>3788</v>
       </c>
@@ -39672,11 +39388,8 @@
       <c r="D89" s="21" t="s">
         <v>3790</v>
       </c>
-      <c r="E89" s="2" t="s">
-        <v>3832</v>
-      </c>
-    </row>
-    <row r="90" spans="1:5">
+    </row>
+    <row r="90" spans="1:4">
       <c r="A90" s="18" t="s">
         <v>3791</v>
       </c>
@@ -39689,11 +39402,8 @@
       <c r="D90" s="21" t="s">
         <v>3728</v>
       </c>
-      <c r="E90" s="2" t="s">
-        <v>3832</v>
-      </c>
-    </row>
-    <row r="91" spans="1:5">
+    </row>
+    <row r="91" spans="1:4">
       <c r="A91" s="18" t="s">
         <v>3793</v>
       </c>
@@ -39706,11 +39416,8 @@
       <c r="D91" s="21" t="s">
         <v>3737</v>
       </c>
-      <c r="E91" s="2" t="s">
-        <v>2543</v>
-      </c>
-    </row>
-    <row r="92" spans="1:5">
+    </row>
+    <row r="92" spans="1:4">
       <c r="A92" s="18" t="s">
         <v>3795</v>
       </c>
@@ -39723,11 +39430,8 @@
       <c r="D92" s="21" t="s">
         <v>536</v>
       </c>
-      <c r="E92" s="2" t="s">
-        <v>3832</v>
-      </c>
-    </row>
-    <row r="93" spans="1:5">
+    </row>
+    <row r="93" spans="1:4">
       <c r="A93" s="18" t="s">
         <v>3797</v>
       </c>
@@ -39740,11 +39444,8 @@
       <c r="D93" s="21" t="s">
         <v>3728</v>
       </c>
-      <c r="E93" s="2" t="s">
-        <v>2543</v>
-      </c>
-    </row>
-    <row r="94" spans="1:5">
+    </row>
+    <row r="94" spans="1:4">
       <c r="A94" s="18" t="s">
         <v>3799</v>
       </c>
@@ -39757,11 +39458,8 @@
       <c r="D94" s="21" t="s">
         <v>3734</v>
       </c>
-      <c r="E94" s="2" t="s">
-        <v>2543</v>
-      </c>
-    </row>
-    <row r="95" spans="1:5">
+    </row>
+    <row r="95" spans="1:4">
       <c r="A95" s="18" t="s">
         <v>3801</v>
       </c>
@@ -39773,9 +39471,6 @@
       </c>
       <c r="D95" s="21" t="s">
         <v>3734</v>
-      </c>
-      <c r="E95" s="2" t="s">
-        <v>2543</v>
       </c>
     </row>
   </sheetData>
@@ -39798,7 +39493,7 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:D952"/>
   <sheetViews>
-    <sheetView view="pageLayout" topLeftCell="A935" zoomScale="70" zoomScaleNormal="130" zoomScaleSheetLayoutView="85" zoomScalePageLayoutView="70" workbookViewId="0">
+    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A875" zoomScale="70" zoomScaleNormal="130" zoomScaleSheetLayoutView="85" zoomScalePageLayoutView="70" workbookViewId="0">
       <selection activeCell="B943" sqref="B943"/>
     </sheetView>
   </sheetViews>

</xml_diff>